<commit_message>
Improved changelog and removed erroneous component
LBS1.2 C6 had a old entry, removed now.
</commit_message>
<xml_diff>
--- a/LoRa Base Station/PCB Files/LBS1.2 Rev1.2 BOM.xlsx
+++ b/LoRa Base Station/PCB Files/LBS1.2 Rev1.2 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\GitHub\Trak-TFRC-System\LoRa Base Station\PCB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C76FDE05-7EA8-440F-A8C3-A944404E9906}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D16AA30B-DCDF-49C1-B09B-70CBC7DB2692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5ABB82E-A1AF-4B43-86DC-B16426612706}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
   <si>
     <t>Qty</t>
   </si>
@@ -178,13 +178,7 @@
     <t>https://www.sunrom.com/p/4k7-1-0805-pack-of-100</t>
   </si>
   <si>
-    <t>4.7uF</t>
-  </si>
-  <si>
     <t>C6</t>
-  </si>
-  <si>
-    <t>https://www.evelta.com/4-7-uf-16v-0805-smd-multi-layer-ceramic-capacitor-0805x475k160ct-walsin/</t>
   </si>
   <si>
     <t>470uF</t>
@@ -888,10 +882,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47106DB8-1B6E-4E8E-BD61-1C857F6A74E1}">
-  <dimension ref="A1:N46"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,21 +902,21 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1">
         <v>10</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -955,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>7</v>
@@ -968,19 +962,19 @@
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A32" si="0">B4*$B$1</f>
+        <f t="shared" ref="A4:A31" si="0">B4*$B$1</f>
         <v>10</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>10</v>
@@ -1009,7 +1003,7 @@
         <v>14</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>15</v>
@@ -1041,7 +1035,7 @@
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
       <c r="H6" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1084,7 +1078,7 @@
         <v>27</v>
       </c>
       <c r="E8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>28</v>
@@ -1111,7 +1105,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>15</v>
@@ -1135,10 +1129,10 @@
         <v>31</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>15</v>
@@ -1147,7 +1141,7 @@
         <v>16</v>
       </c>
       <c r="H10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -1261,13 +1255,13 @@
         <v>1</v>
       </c>
       <c r="C15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>132</v>
-      </c>
-      <c r="D15" t="s">
-        <v>133</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>134</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>28</v>
@@ -1276,7 +1270,7 @@
         <v>29</v>
       </c>
       <c r="H15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1288,13 +1282,13 @@
         <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>28</v>
@@ -1303,7 +1297,7 @@
         <v>29</v>
       </c>
       <c r="H16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,22 +1309,20 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>129</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -1342,20 +1334,18 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>24</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -1363,97 +1353,98 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B19" s="3">
-        <v>1</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>55</v>
+      <c r="B19" s="11">
+        <v>1</v>
+      </c>
+      <c r="C19" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="D19" t="s">
+        <v>128</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
-        <v>57</v>
-      </c>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B20" s="11">
-        <v>1</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="D20" t="s">
-        <v>130</v>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
+        <v>56</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>127</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>140</v>
+      </c>
+      <c r="D21" t="s">
+        <v>141</v>
+      </c>
+      <c r="E21" t="s">
+        <v>142</v>
+      </c>
+      <c r="F21" t="s">
+        <v>143</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="H21" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B22" s="3">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" t="s">
-        <v>143</v>
-      </c>
-      <c r="E22" t="s">
-        <v>144</v>
-      </c>
-      <c r="F22" t="s">
-        <v>145</v>
+        <v>1</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>62</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>146</v>
+        <v>108</v>
       </c>
       <c r="H22" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1465,19 +1456,20 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>109</v>
+        <v>64</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H23" t="s">
-        <v>111</v>
+        <v>65</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -1489,68 +1481,66 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>68</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F25" s="3"/>
+        <v>99</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>74</v>
+      </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B26" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>75</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="D26" s="3"/>
       <c r="E26" s="3" t="s">
         <v>101</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>77</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -1561,19 +1551,21 @@
       <c r="B27" s="3">
         <v>1</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D27" s="3"/>
+      <c r="C27" t="s">
+        <v>137</v>
+      </c>
+      <c r="D27" t="s">
+        <v>138</v>
+      </c>
       <c r="E27" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F27" s="3" t="s">
         <v>76</v>
+      </c>
+      <c r="F27" t="s">
+        <v>139</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>102</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -1584,188 +1576,182 @@
       <c r="B28" s="3">
         <v>1</v>
       </c>
-      <c r="C28" t="s">
-        <v>139</v>
-      </c>
-      <c r="D28" t="s">
-        <v>140</v>
+      <c r="C28" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>79</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F28" t="s">
-        <v>141</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="F28" s="3"/>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B29" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="E29" s="3" t="s">
         <v>82</v>
+      </c>
+      <c r="D29" t="s">
+        <v>120</v>
+      </c>
+      <c r="E29" t="s">
+        <v>121</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="3" t="s">
-        <v>83</v>
+      <c r="H29" s="9" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B30" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C30" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D30" t="s">
-        <v>122</v>
-      </c>
-      <c r="E30" t="s">
-        <v>123</v>
+      <c r="E30" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="9" t="s">
-        <v>124</v>
+      <c r="H30" s="3" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>87</v>
+        <v>20</v>
+      </c>
+      <c r="B31" s="11">
+        <v>2</v>
+      </c>
+      <c r="C31" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="D31" t="s">
+        <v>146</v>
+      </c>
+      <c r="E31" t="s">
+        <v>147</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>88</v>
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B32" s="11">
-        <v>2</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="D32" t="s">
-        <v>148</v>
-      </c>
-      <c r="E32" t="s">
-        <v>149</v>
-      </c>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3" t="s">
-        <v>150</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="2" t="s">
+        <v>117</v>
+      </c>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B34" s="3"/>
-      <c r="C34" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="E34" s="3"/>
+      <c r="A34">
+        <f>B34*$B$1</f>
+        <v>10</v>
+      </c>
+      <c r="B34" s="3">
+        <v>1</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>B35*$B$1</f>
-        <v>10</v>
-      </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3" t="s">
-        <v>63</v>
+        <v>20</v>
+      </c>
+      <c r="B35" s="4">
+        <v>2</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N35" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <f>B36*$B$1</f>
-        <v>20</v>
-      </c>
-      <c r="B36" s="4">
-        <v>2</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="N36" t="s">
-        <v>118</v>
-      </c>
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="4"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="4"/>
-      <c r="B37" s="4"/>
-      <c r="C37" s="5" t="s">
-        <v>94</v>
+      <c r="A37" s="4">
+        <f>B37*$B$1</f>
+        <v>10</v>
+      </c>
+      <c r="B37" s="4">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6" t="s">
+        <v>93</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="4"/>
+      <c r="H37" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -1776,84 +1762,82 @@
         <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="10" t="s">
-        <v>106</v>
-      </c>
+      <c r="H38" s="4"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
-        <f>B39*$B$1</f>
-        <v>10</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
+      <c r="A39" s="4"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="C40" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
       <c r="H40" s="4"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="4"/>
-      <c r="B41" s="4"/>
-      <c r="C41" s="5" t="s">
-        <v>90</v>
+      <c r="A41" s="4">
+        <f t="shared" ref="A41:A44" si="1">B41*$B$1</f>
+        <v>10</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6" t="s">
+        <v>89</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="4"/>
+      <c r="H41" s="10" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <f t="shared" ref="A42:A45" si="1">B42*$B$1</f>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>20</v>
       </c>
       <c r="B42" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="10" t="s">
-        <v>107</v>
-      </c>
+      <c r="H42" s="4"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f t="shared" si="1"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B43" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1866,52 +1850,35 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B44" s="4">
-        <v>1</v>
-      </c>
-      <c r="C44" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D44" s="5"/>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
+      <c r="B44" s="8">
+        <v>1</v>
+      </c>
+      <c r="C44" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
-        <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-      <c r="B45" s="8">
-        <v>1</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>105</v>
-      </c>
+      <c r="A45" s="4"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="4"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="5"/>
+      <c r="G45" s="4"/>
       <c r="H45" s="4"/>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" s="4"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C42" r:id="rId1" xr:uid="{05C5DF2F-E63D-4B94-80E8-83AAAD9A1FE3}"/>
-    <hyperlink ref="C43" r:id="rId2" xr:uid="{D553B020-4A28-4132-9C24-BB15A690582C}"/>
-    <hyperlink ref="C44" r:id="rId3" xr:uid="{E6A3B0D8-88A5-4C5D-B93B-2C6A998B0887}"/>
-    <hyperlink ref="C38" r:id="rId4" xr:uid="{A6C34D53-A2E0-4747-A04F-7B7984A43EC7}"/>
-    <hyperlink ref="C39" r:id="rId5" xr:uid="{D6F2ECEF-590F-48E9-8EB8-35D5F53D7E8C}"/>
+    <hyperlink ref="C41" r:id="rId1" xr:uid="{05C5DF2F-E63D-4B94-80E8-83AAAD9A1FE3}"/>
+    <hyperlink ref="C42" r:id="rId2" xr:uid="{D553B020-4A28-4132-9C24-BB15A690582C}"/>
+    <hyperlink ref="C43" r:id="rId3" xr:uid="{E6A3B0D8-88A5-4C5D-B93B-2C6A998B0887}"/>
+    <hyperlink ref="C37" r:id="rId4" xr:uid="{A6C34D53-A2E0-4747-A04F-7B7984A43EC7}"/>
+    <hyperlink ref="C38" r:id="rId5" xr:uid="{D6F2ECEF-590F-48E9-8EB8-35D5F53D7E8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>

</xml_diff>

<commit_message>
Updated MC and LBS
LBS1.2 to 1.3
MC1.1 to 1.2
Added 470R resistors to mosfets to limit inrush
</commit_message>
<xml_diff>
--- a/LoRa Base Station/PCB Files/LBS1.2 Rev1.2 BOM.xlsx
+++ b/LoRa Base Station/PCB Files/LBS1.2 Rev1.2 BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Storage\Documents\GitHub\Trak-TFRC-System\LoRa Base Station\PCB Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50D994C-5227-4C9E-8000-FDAFE0D02B28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281CAD7D-2461-41EE-9AC3-0DC924C74740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D5ABB82E-A1AF-4B43-86DC-B16426612706}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="154">
   <si>
     <t>Qty</t>
   </si>
@@ -485,6 +485,15 @@
   </si>
   <si>
     <t>EN, BOOT</t>
+  </si>
+  <si>
+    <t>470R</t>
+  </si>
+  <si>
+    <t>https://www.sunrom.com/p/470r-1-0805-pack-of-100</t>
+  </si>
+  <si>
+    <t>R15</t>
   </si>
 </sst>
 </file>
@@ -882,10 +891,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47106DB8-1B6E-4E8E-BD61-1C857F6A74E1}">
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:AM46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -967,7 +976,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A31" si="0">B4*$B$1</f>
+        <f t="shared" ref="A4:A32" si="0">B4*$B$1</f>
         <v>10</v>
       </c>
       <c r="B4" s="3">
@@ -1300,7 +1309,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1309,218 +1318,247 @@
         <v>1</v>
       </c>
       <c r="C17" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+      <c r="M17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3"/>
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+      <c r="V17" s="3"/>
+      <c r="W17" s="3"/>
+      <c r="X17" s="3"/>
+      <c r="Y17" s="3"/>
+      <c r="Z17" s="3"/>
+      <c r="AA17" s="3"/>
+      <c r="AB17" s="3"/>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
+      <c r="AG17" s="3"/>
+      <c r="AH17" s="3"/>
+      <c r="AI17" s="3"/>
+      <c r="AJ17" s="3"/>
+      <c r="AK17" s="3"/>
+      <c r="AL17" s="3"/>
+      <c r="AM17" s="3"/>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E18" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="3"/>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B19" s="11">
-        <v>1</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="D19" t="s">
-        <v>127</v>
+      <c r="B19" s="3">
+        <v>1</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H19" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
+      <c r="B20" s="11">
+        <v>1</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" t="s">
+        <v>127</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E21" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F21" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="G20" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="H20" t="s">
+      <c r="H21" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B22" s="3">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C22" t="s">
         <v>139</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D22" t="s">
         <v>140</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E22" t="s">
         <v>141</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F22" t="s">
         <v>142</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="H21" t="s">
+      <c r="H22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G22" s="3" t="s">
+      <c r="G23" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H22" t="s">
+      <c r="H23" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E24" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="F24" s="3"/>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>74</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="F25" s="3"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1529,46 +1567,46 @@
         <v>2</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="D26" s="3"/>
+        <v>72</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E26" s="3" t="s">
-        <v>150</v>
+        <v>99</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>74</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>136</v>
-      </c>
-      <c r="D27" t="s">
-        <v>137</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D27" s="3"/>
       <c r="E27" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F27" t="s">
-        <v>138</v>
+        <v>150</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>74</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1576,182 +1614,188 @@
       <c r="B28" s="3">
         <v>1</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>79</v>
+      <c r="C28" t="s">
+        <v>136</v>
+      </c>
+      <c r="D28" t="s">
+        <v>137</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F28" s="3"/>
+        <v>76</v>
+      </c>
+      <c r="F28" t="s">
+        <v>138</v>
+      </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="B29" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D29" t="s">
-        <v>119</v>
-      </c>
-      <c r="E29" t="s">
-        <v>120</v>
+        <v>78</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>80</v>
       </c>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
-      <c r="H29" s="9" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H29" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B30" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
+      </c>
+      <c r="D30" t="s">
+        <v>119</v>
+      </c>
+      <c r="E30" t="s">
+        <v>120</v>
       </c>
       <c r="F30" s="3"/>
       <c r="G30" s="3"/>
-      <c r="H30" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H30" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B31" s="11">
-        <v>2</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="D31" t="s">
-        <v>145</v>
-      </c>
-      <c r="E31" t="s">
-        <v>146</v>
+        <v>10</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B32" s="11">
+        <v>2</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D32" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
-      <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B33" s="3"/>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="3"/>
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B34" s="3"/>
+      <c r="C34" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="E33" s="3"/>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <f>B34*$B$1</f>
-        <v>10</v>
-      </c>
-      <c r="B34" s="3">
-        <v>1</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3" t="s">
-        <v>61</v>
-      </c>
+      <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <f>B35*$B$1</f>
+        <v>10</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="F35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f>B36*$B$1</f>
         <v>20</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B36" s="4">
         <v>2</v>
       </c>
-      <c r="C35" s="4" t="s">
+      <c r="C36" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D36" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E36" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F36" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="H35" s="4" t="s">
+      <c r="H36" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="N35" t="s">
+      <c r="N36" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="4"/>
-      <c r="B36" s="4"/>
-      <c r="C36" s="5" t="s">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="5" t="s">
         <v>92</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="4"/>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
-        <f>B37*$B$1</f>
-        <v>10</v>
-      </c>
-      <c r="B37" s="4">
-        <v>1</v>
-      </c>
-      <c r="C37" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
-      <c r="H37" s="10" t="s">
-        <v>103</v>
-      </c>
+      <c r="H37" s="4"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
@@ -1762,82 +1806,84 @@
         <v>1</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D38" s="5"/>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
-      <c r="H38" s="4"/>
+      <c r="H38" s="10" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="4"/>
-      <c r="B39" s="4"/>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="A39" s="4">
+        <f>B39*$B$1</f>
+        <v>10</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
       <c r="H39" s="4"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="5" t="s">
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4"/>
+      <c r="C41" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="5"/>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="4"/>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
-        <f t="shared" ref="A41:A44" si="1">B41*$B$1</f>
-        <v>10</v>
-      </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="6" t="s">
-        <v>89</v>
       </c>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
-      <c r="H41" s="10" t="s">
-        <v>104</v>
-      </c>
+      <c r="H41" s="4"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
-        <f t="shared" si="1"/>
-        <v>20</v>
+        <f t="shared" ref="A42:A45" si="1">B42*$B$1</f>
+        <v>10</v>
       </c>
       <c r="B42" s="4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="5"/>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
-      <c r="H42" s="4"/>
+      <c r="H42" s="10" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B43" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D43" s="5"/>
       <c r="E43" s="5"/>
@@ -1850,35 +1896,52 @@
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B44" s="8">
-        <v>1</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
+      <c r="B44" s="4">
+        <v>1</v>
+      </c>
+      <c r="C44" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" s="4"/>
-      <c r="B45" s="4"/>
-      <c r="C45" s="4"/>
+      <c r="A45" s="4">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="B45" s="8">
+        <v>1</v>
+      </c>
+      <c r="C45" s="7" t="s">
+        <v>102</v>
+      </c>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="G45" s="5"/>
       <c r="H45" s="4"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C41" r:id="rId1" xr:uid="{05C5DF2F-E63D-4B94-80E8-83AAAD9A1FE3}"/>
-    <hyperlink ref="C42" r:id="rId2" xr:uid="{D553B020-4A28-4132-9C24-BB15A690582C}"/>
-    <hyperlink ref="C43" r:id="rId3" xr:uid="{E6A3B0D8-88A5-4C5D-B93B-2C6A998B0887}"/>
-    <hyperlink ref="C37" r:id="rId4" xr:uid="{A6C34D53-A2E0-4747-A04F-7B7984A43EC7}"/>
-    <hyperlink ref="C38" r:id="rId5" xr:uid="{D6F2ECEF-590F-48E9-8EB8-35D5F53D7E8C}"/>
+    <hyperlink ref="C42" r:id="rId1" xr:uid="{05C5DF2F-E63D-4B94-80E8-83AAAD9A1FE3}"/>
+    <hyperlink ref="C43" r:id="rId2" xr:uid="{D553B020-4A28-4132-9C24-BB15A690582C}"/>
+    <hyperlink ref="C44" r:id="rId3" xr:uid="{E6A3B0D8-88A5-4C5D-B93B-2C6A998B0887}"/>
+    <hyperlink ref="C38" r:id="rId4" xr:uid="{A6C34D53-A2E0-4747-A04F-7B7984A43EC7}"/>
+    <hyperlink ref="C39" r:id="rId5" xr:uid="{D6F2ECEF-590F-48E9-8EB8-35D5F53D7E8C}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId6"/>

</xml_diff>